<commit_message>
-modified the import methods in the InvestmentBudgetsService to account for an additional criteria worksheet -added an interface for the ExpressionValidationService and added an additional method to validate critera without getting a results count -added an additional form data parameter to include the user criteria when checking criteria during an budget import
</commit_message>
<xml_diff>
--- a/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestInvestmentBudgets.xlsx
+++ b/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestInvestmentBudgets.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\iAM\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\TestData\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\iAM\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\TestUtils\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB0C478F-EDDC-4205-990F-D070C9925E73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D30CCA-36D4-4A25-99C2-FF23219343DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Budget" sheetId="1" r:id="rId1"/>
+    <sheet name="Criteria" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Year</t>
   </si>
@@ -29,6 +30,18 @@
   </si>
   <si>
     <t>Sample Budget 2</t>
+  </si>
+  <si>
+    <t>BUDGET_NAME</t>
+  </si>
+  <si>
+    <t>CRITERIA</t>
+  </si>
+  <si>
+    <t>[INTERSTATE]=|Y| AND [INTERNETREPORT]=|State|</t>
+  </si>
+  <si>
+    <t>[INTERSTATE]='Y' AND [INTERNETREPORT]='State'</t>
   </si>
 </sst>
 </file>
@@ -64,9 +77,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -418,4 +432,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DCA90F-D7C2-4289-BDBA-06CE9ECE1DB1}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Grab from other branch changes that fixed two more tests. No failures here.
</commit_message>
<xml_diff>
--- a/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestInvestmentBudgets.xlsx
+++ b/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestInvestmentBudgets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aborgaonkar\source\repos\Infrastructure Asset Management\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\TestUtils\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Infrastructure Asset Management\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\TestUtils\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816201BE-BDE3-4919-A17E-01DBAD9670B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4219CD4C-B6E6-493F-A686-0663224D76F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1956" yWindow="-24" windowWidth="16980" windowHeight="12324" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="1" r:id="rId1"/>
@@ -38,10 +38,10 @@
     <t>CRITERIA</t>
   </si>
   <si>
-    <t>[INTERSTATE]=|Y| AND [INTERNETREPORT]=|State|</t>
-  </si>
-  <si>
-    <t>[INTERSTATE]='Y' AND [INTERNETREPORT]='State'</t>
+    <t>[INTERSTATE]=|Y| AND [INTERNET_REPORT]=|State|</t>
+  </si>
+  <si>
+    <t>[INTERSTATE]='Y' AND [INTERNET_REPORT]='State'</t>
   </si>
 </sst>
 </file>
@@ -77,10 +77,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,13 +397,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -420,7 +419,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B2" s="1">
         <v>5000000</v>
@@ -439,13 +438,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -460,7 +459,7 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -468,7 +467,7 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Note which tests are issues
</commit_message>
<xml_diff>
--- a/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestInvestmentBudgets.xlsx
+++ b/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestInvestmentBudgets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Infrastructure Asset Management\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\TestUtils\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4219CD4C-B6E6-493F-A686-0663224D76F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CF2127-533E-466E-8403-F41C69C25288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1956" yWindow="-24" windowWidth="16980" windowHeight="12324" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2856" yWindow="36" windowWidth="20184" windowHeight="12324" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -419,7 +419,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B2" s="1">
         <v>5000000</v>

</xml_diff>

<commit_message>
Set spreadsheet to 2023. No failures.
</commit_message>
<xml_diff>
--- a/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestInvestmentBudgets.xlsx
+++ b/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestInvestmentBudgets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Infrastructure Asset Management\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\TestUtils\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CF2127-533E-466E-8403-F41C69C25288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6156A2E2-FDA8-4352-A1E4-25BD83BBBCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2856" yWindow="36" windowWidth="20184" windowHeight="12324" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,7 +397,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -419,7 +419,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B2" s="1">
         <v>5000000</v>

</xml_diff>

<commit_message>
Everything is behaving with both tests and spreadsheet set to 2022.
</commit_message>
<xml_diff>
--- a/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestInvestmentBudgets.xlsx
+++ b/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestInvestmentBudgets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Infrastructure Asset Management\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\TestUtils\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6156A2E2-FDA8-4352-A1E4-25BD83BBBCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91032C5C-B23B-425E-AE0D-8B700F41045D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2856" yWindow="36" windowWidth="20184" windowHeight="12324" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4416" yWindow="324" windowWidth="20184" windowHeight="12324" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -419,7 +419,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B2" s="1">
         <v>5000000</v>

</xml_diff>